<commit_message>
clean python loader code by using only pandas to read excel file; remove unneeded old templates
</commit_message>
<xml_diff>
--- a/data/20170127_GEP00001/20170127_GEP00001.xlsx
+++ b/data/20170127_GEP00001/20170127_GEP00001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -1612,7 +1612,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1696,7 +1696,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1791,7 +1791,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1936,14 +1936,14 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2339,23 +2339,25 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="12" style="0" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="31.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="31.77"/>
@@ -3291,8 +3293,8 @@
   </sheetPr>
   <dimension ref="A1:I577"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A474" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16968,7 +16970,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17265,7 +17267,7 @@
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20105,7 +20107,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20116,7 +20118,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>

</xml_diff>

<commit_message>
updates for loading project 1 & 2; missing data for loading project 3
</commit_message>
<xml_diff>
--- a/data/20170127_GEP00001/20170127_GEP00001.xlsx
+++ b/data/20170127_GEP00001/20170127_GEP00001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,6 @@
     <sheet name="ExperimentLayout" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Plate" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="SequencingLibrary" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Results" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="469">
   <si>
     <t xml:space="preserve">geid</t>
   </si>
@@ -1435,48 +1434,6 @@
   </si>
   <si>
     <t xml:space="preserve">GE-P6B4-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_clone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_indel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_aminoacid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_impactonprotein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results_growthrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracking_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">which clones are delivered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e.g. frameshift. This could be a ‘notes’ field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICW data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incucyte data, slope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked to tab ‘Tracking’</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1541,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1668,7 +1625,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1763,7 +1720,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1909,8 +1866,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2312,8 +2269,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2899,8 +2856,8 @@
   </sheetPr>
   <dimension ref="A1:I577"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16575,8 +16532,8 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16872,8 +16829,8 @@
   </sheetPr>
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19703,116 +19660,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected errors in well names in SequencingLibrary tab
</commit_message>
<xml_diff>
--- a/data/20170127_GEP00001/20170127_GEP00001.xlsx
+++ b/data/20170127_GEP00001/20170127_GEP00001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -791,6 +791,18 @@
     <t xml:space="preserve">Fluidigm</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1B10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1B11-C</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0193</t>
   </si>
   <si>
@@ -827,16 +839,16 @@
     <t xml:space="preserve">GE-P1B9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1B10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1B11-C</t>
+    <t xml:space="preserve">FLD0207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1C10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1C11-C</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0201</t>
@@ -851,6 +863,15 @@
     <t xml:space="preserve">GE-P1C5-C</t>
   </si>
   <si>
+    <t xml:space="preserve">gDNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1C5-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0203</t>
   </si>
   <si>
@@ -875,16 +896,10 @@
     <t xml:space="preserve">GE-P1C9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0207</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1C10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1C11-C</t>
+    <t xml:space="preserve">FLD0296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1C9-G</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0209</t>
@@ -893,6 +908,12 @@
     <t xml:space="preserve">GE-P1E2-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P1E2-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0210</t>
   </si>
   <si>
@@ -935,6 +956,24 @@
     <t xml:space="preserve">GE-P1E9-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P6B4-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2D10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2D11-C</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0217</t>
   </si>
   <si>
@@ -971,16 +1010,22 @@
     <t xml:space="preserve">GE-P2D9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2D10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2D11-C</t>
+    <t xml:space="preserve">FLD0298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2D9-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2E10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2E11-C</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0225</t>
@@ -1019,16 +1064,16 @@
     <t xml:space="preserve">GE-P2E9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2E10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2E11-C</t>
+    <t xml:space="preserve">FLD0239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2F10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2F11-C</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0233</t>
@@ -1061,22 +1106,28 @@
     <t xml:space="preserve">GE-P2F8-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P2F8-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0238</t>
   </si>
   <si>
     <t xml:space="preserve">GE-P2F9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2F10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2F11-C</t>
+    <t xml:space="preserve">FLD0247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3B10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3B11-C</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0241</t>
@@ -1115,16 +1166,10 @@
     <t xml:space="preserve">GE-P3B9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3B10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3B11-C</t>
+    <t xml:space="preserve">FLD0290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3B9-G</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0249</t>
@@ -1139,6 +1184,12 @@
     <t xml:space="preserve">GE-P3C3-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3C3-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0251</t>
   </si>
   <si>
@@ -1175,6 +1226,18 @@
     <t xml:space="preserve">GE-P3C9-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3D10-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLD0264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3D11-C</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0257</t>
   </si>
   <si>
@@ -1211,16 +1274,10 @@
     <t xml:space="preserve">GE-P3D9-C</t>
   </si>
   <si>
-    <t xml:space="preserve">FLD0263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3D10-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3D11-C</t>
+    <t xml:space="preserve">FLD0292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P3D9-G</t>
   </si>
   <si>
     <t xml:space="preserve">FLD0265</t>
@@ -1247,12 +1304,24 @@
     <t xml:space="preserve">GE-P4B5-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P4B5-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0269</t>
   </si>
   <si>
     <t xml:space="preserve">GE-P4B6-C</t>
   </si>
   <si>
+    <t xml:space="preserve">FLD0294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE-P4B6-G</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLD0270</t>
   </si>
   <si>
@@ -1365,75 +1434,6 @@
   </si>
   <si>
     <t xml:space="preserve">GE-P4D9-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gDNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0290</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3B9-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3C3-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P3D9-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P4B5-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P4B6-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1C5-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1C9-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0297</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P1E2-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2D9-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P2F8-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLD0300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE-P6B4-G</t>
   </si>
 </sst>
 </file>
@@ -1541,18 +1541,18 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1610,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1625,17 +1625,17 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,7 +1705,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1720,17 +1720,17 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1851,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1866,15 +1866,15 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,7 +2254,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2269,29 +2269,27 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="11" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="31.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="11" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="24" min="22" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2839,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2856,19 +2854,19 @@
   </sheetPr>
   <dimension ref="A1:I577"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G113" activeCellId="0" sqref="G113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16517,7 +16515,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -16532,17 +16530,17 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="73.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16814,7 +16812,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -16829,18 +16827,18 @@
   </sheetPr>
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16874,7 +16872,7 @@
         <v>111</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>251</v>
@@ -16900,7 +16898,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>251</v>
@@ -16926,7 +16924,7 @@
         <v>111</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>251</v>
@@ -16952,7 +16950,7 @@
         <v>111</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>251</v>
@@ -16978,7 +16976,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>251</v>
@@ -17004,7 +17002,7 @@
         <v>111</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>251</v>
@@ -17030,7 +17028,7 @@
         <v>111</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>251</v>
@@ -17056,7 +17054,7 @@
         <v>111</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>251</v>
@@ -17082,7 +17080,7 @@
         <v>111</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>251</v>
@@ -17108,7 +17106,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>251</v>
@@ -17134,7 +17132,7 @@
         <v>111</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>251</v>
@@ -17160,7 +17158,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>251</v>
@@ -17186,10 +17184,10 @@
         <v>111</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>252</v>
@@ -17201,10 +17199,10 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17212,7 +17210,7 @@
         <v>111</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>251</v>
@@ -17227,10 +17225,10 @@
         <v>10</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17238,7 +17236,7 @@
         <v>111</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>251</v>
@@ -17253,10 +17251,10 @@
         <v>10</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17264,7 +17262,7 @@
         <v>111</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>251</v>
@@ -17279,10 +17277,10 @@
         <v>10</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17290,7 +17288,7 @@
         <v>111</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>251</v>
@@ -17305,10 +17303,10 @@
         <v>10</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17316,10 +17314,10 @@
         <v>111</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>252</v>
@@ -17331,10 +17329,10 @@
         <v>10</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17342,7 +17340,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>251</v>
@@ -17357,10 +17355,10 @@
         <v>10</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17368,10 +17366,10 @@
         <v>111</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>252</v>
@@ -17383,10 +17381,10 @@
         <v>10</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17394,7 +17392,7 @@
         <v>111</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>251</v>
@@ -17409,10 +17407,10 @@
         <v>10</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17420,7 +17418,7 @@
         <v>111</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>251</v>
@@ -17435,10 +17433,10 @@
         <v>10</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17446,7 +17444,7 @@
         <v>111</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>251</v>
@@ -17461,10 +17459,10 @@
         <v>10</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17472,7 +17470,7 @@
         <v>111</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>251</v>
@@ -17487,18 +17485,18 @@
         <v>10</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>251</v>
@@ -17513,18 +17511,18 @@
         <v>10</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>251</v>
@@ -17539,18 +17537,18 @@
         <v>10</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>251</v>
@@ -17565,21 +17563,21 @@
         <v>10</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>252</v>
@@ -17591,10 +17589,10 @@
         <v>10</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17602,7 +17600,7 @@
         <v>213</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>251</v>
@@ -17617,10 +17615,10 @@
         <v>10</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17628,7 +17626,7 @@
         <v>213</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>251</v>
@@ -17643,10 +17641,10 @@
         <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17654,7 +17652,7 @@
         <v>213</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>251</v>
@@ -17669,10 +17667,10 @@
         <v>10</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17680,7 +17678,7 @@
         <v>213</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>251</v>
@@ -17695,10 +17693,10 @@
         <v>10</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17706,7 +17704,7 @@
         <v>213</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>251</v>
@@ -17721,10 +17719,10 @@
         <v>10</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17732,7 +17730,7 @@
         <v>213</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>251</v>
@@ -17747,10 +17745,10 @@
         <v>10</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17758,7 +17756,7 @@
         <v>213</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>251</v>
@@ -17773,10 +17771,10 @@
         <v>10</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17784,7 +17782,7 @@
         <v>213</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>251</v>
@@ -17799,10 +17797,10 @@
         <v>10</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17810,10 +17808,10 @@
         <v>213</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>252</v>
@@ -17825,10 +17823,10 @@
         <v>10</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17836,7 +17834,7 @@
         <v>213</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>251</v>
@@ -17851,10 +17849,10 @@
         <v>10</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17862,7 +17860,7 @@
         <v>213</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>251</v>
@@ -17877,10 +17875,10 @@
         <v>10</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17888,7 +17886,7 @@
         <v>213</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>251</v>
@@ -17903,10 +17901,10 @@
         <v>10</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17914,7 +17912,7 @@
         <v>213</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>251</v>
@@ -17929,10 +17927,10 @@
         <v>10</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17940,7 +17938,7 @@
         <v>213</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>251</v>
@@ -17955,10 +17953,10 @@
         <v>10</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17966,7 +17964,7 @@
         <v>213</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>251</v>
@@ -17981,10 +17979,10 @@
         <v>10</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17992,7 +17990,7 @@
         <v>213</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>251</v>
@@ -18007,10 +18005,10 @@
         <v>10</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18018,7 +18016,7 @@
         <v>213</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>251</v>
@@ -18033,10 +18031,10 @@
         <v>10</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18044,7 +18042,7 @@
         <v>213</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>251</v>
@@ -18059,10 +18057,10 @@
         <v>10</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18070,7 +18068,7 @@
         <v>213</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>251</v>
@@ -18085,10 +18083,10 @@
         <v>10</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18096,7 +18094,7 @@
         <v>213</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>251</v>
@@ -18111,18 +18109,18 @@
         <v>10</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>251</v>
@@ -18137,18 +18135,18 @@
         <v>10</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>251</v>
@@ -18163,18 +18161,18 @@
         <v>10</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>251</v>
@@ -18189,18 +18187,18 @@
         <v>10</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>251</v>
@@ -18215,21 +18213,21 @@
         <v>10</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>252</v>
@@ -18241,18 +18239,18 @@
         <v>10</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>251</v>
@@ -18267,10 +18265,10 @@
         <v>10</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18278,7 +18276,7 @@
         <v>214</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>251</v>
@@ -18293,10 +18291,10 @@
         <v>10</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18304,7 +18302,7 @@
         <v>214</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>251</v>
@@ -18319,10 +18317,10 @@
         <v>10</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18330,7 +18328,7 @@
         <v>214</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>251</v>
@@ -18345,10 +18343,10 @@
         <v>10</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18356,7 +18354,7 @@
         <v>214</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>251</v>
@@ -18371,10 +18369,10 @@
         <v>10</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18382,7 +18380,7 @@
         <v>214</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>251</v>
@@ -18397,10 +18395,10 @@
         <v>10</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18408,7 +18406,7 @@
         <v>214</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>251</v>
@@ -18423,10 +18421,10 @@
         <v>10</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18434,7 +18432,7 @@
         <v>214</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>251</v>
@@ -18449,10 +18447,10 @@
         <v>10</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18460,7 +18458,7 @@
         <v>214</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>251</v>
@@ -18475,10 +18473,10 @@
         <v>10</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18486,10 +18484,10 @@
         <v>214</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>252</v>
@@ -18501,10 +18499,10 @@
         <v>10</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18512,7 +18510,7 @@
         <v>214</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>251</v>
@@ -18527,10 +18525,10 @@
         <v>10</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18538,7 +18536,7 @@
         <v>214</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>251</v>
@@ -18553,10 +18551,10 @@
         <v>10</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18564,10 +18562,10 @@
         <v>214</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>252</v>
@@ -18579,10 +18577,10 @@
         <v>10</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18590,7 +18588,7 @@
         <v>214</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>251</v>
@@ -18605,10 +18603,10 @@
         <v>10</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18616,7 +18614,7 @@
         <v>214</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>251</v>
@@ -18631,10 +18629,10 @@
         <v>10</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18642,7 +18640,7 @@
         <v>214</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>251</v>
@@ -18657,10 +18655,10 @@
         <v>10</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18668,7 +18666,7 @@
         <v>214</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>251</v>
@@ -18683,10 +18681,10 @@
         <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18694,7 +18692,7 @@
         <v>214</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>251</v>
@@ -18709,10 +18707,10 @@
         <v>10</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18720,7 +18718,7 @@
         <v>214</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>251</v>
@@ -18735,18 +18733,18 @@
         <v>10</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>251</v>
@@ -18761,18 +18759,18 @@
         <v>10</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>251</v>
@@ -18787,18 +18785,18 @@
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>251</v>
@@ -18813,18 +18811,18 @@
         <v>10</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>251</v>
@@ -18839,18 +18837,18 @@
         <v>10</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>251</v>
@@ -18865,18 +18863,18 @@
         <v>10</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>251</v>
@@ -18891,18 +18889,18 @@
         <v>10</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>251</v>
@@ -18917,18 +18915,18 @@
         <v>10</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>251</v>
@@ -18943,21 +18941,21 @@
         <v>10</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>252</v>
@@ -18969,10 +18967,10 @@
         <v>10</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18980,7 +18978,7 @@
         <v>215</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>251</v>
@@ -18995,10 +18993,10 @@
         <v>10</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19006,7 +19004,7 @@
         <v>215</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>251</v>
@@ -19021,10 +19019,10 @@
         <v>10</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19032,7 +19030,7 @@
         <v>215</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>251</v>
@@ -19047,10 +19045,10 @@
         <v>10</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19058,7 +19056,7 @@
         <v>215</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>251</v>
@@ -19073,10 +19071,10 @@
         <v>10</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19084,10 +19082,10 @@
         <v>215</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>252</v>
@@ -19099,10 +19097,10 @@
         <v>10</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19110,7 +19108,7 @@
         <v>215</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>251</v>
@@ -19125,10 +19123,10 @@
         <v>10</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19136,10 +19134,10 @@
         <v>215</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>252</v>
@@ -19151,10 +19149,10 @@
         <v>10</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19162,7 +19160,7 @@
         <v>215</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>251</v>
@@ -19177,10 +19175,10 @@
         <v>10</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19188,7 +19186,7 @@
         <v>215</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>251</v>
@@ -19203,10 +19201,10 @@
         <v>10</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19214,7 +19212,7 @@
         <v>215</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>251</v>
@@ -19229,10 +19227,10 @@
         <v>10</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19240,7 +19238,7 @@
         <v>215</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>251</v>
@@ -19255,10 +19253,10 @@
         <v>10</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19266,7 +19264,7 @@
         <v>215</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>251</v>
@@ -19281,10 +19279,10 @@
         <v>10</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19292,7 +19290,7 @@
         <v>215</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>251</v>
@@ -19307,10 +19305,10 @@
         <v>10</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H95" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19318,7 +19316,7 @@
         <v>215</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>251</v>
@@ -19333,10 +19331,10 @@
         <v>10</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19344,7 +19342,7 @@
         <v>215</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>251</v>
@@ -19359,21 +19357,21 @@
         <v>10</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H97" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>252</v>
@@ -19393,13 +19391,13 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>252</v>
@@ -19419,13 +19417,13 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>252</v>
@@ -19448,10 +19446,10 @@
         <v>215</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>252</v>
@@ -19474,10 +19472,10 @@
         <v>215</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>252</v>
@@ -19497,13 +19495,13 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>252</v>
@@ -19523,13 +19521,13 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>252</v>
@@ -19549,13 +19547,13 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>252</v>
@@ -19575,13 +19573,13 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>252</v>
@@ -19601,13 +19599,13 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>252</v>
@@ -19627,13 +19625,13 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>252</v>
@@ -19654,7 +19652,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>